<commit_message>
Started defining Encyclopedia, Knowledge System Models
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandersa\PyCharmProjects\Jupyter-Notebooks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9765"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,20 +46,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,16 +82,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -109,18 +106,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -135,44 +124,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -199,32 +188,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -251,24 +222,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -280,157 +233,178 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -473,22 +447,22 @@
         <v>172.846</v>
       </c>
       <c r="E2">
-        <v>-0.74099999999999999</v>
+        <v>-0.741</v>
       </c>
       <c r="F2">
-        <v>173.85599999999999</v>
+        <v>173.856</v>
       </c>
       <c r="G2">
-        <v>1.47E-2</v>
+        <v>0.0147</v>
       </c>
       <c r="H2">
         <v>0.103989</v>
       </c>
       <c r="I2">
-        <v>5.4299999999999999E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00543</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -499,25 +473,25 @@
         <v>0.01</v>
       </c>
       <c r="D3">
-        <v>172.86699999999999</v>
+        <v>172.867</v>
       </c>
       <c r="E3">
         <v>-0.747</v>
       </c>
       <c r="F3">
-        <v>174.03399999999999</v>
+        <v>174.034</v>
       </c>
       <c r="G3">
-        <v>1.473E-2</v>
+        <v>0.01473</v>
       </c>
       <c r="H3">
         <v>0.103982</v>
       </c>
       <c r="I3">
-        <v>5.4200000000000003E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00542</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -537,16 +511,16 @@
         <v>173.679</v>
       </c>
       <c r="G4">
-        <v>1.4789999999999999E-2</v>
+        <v>0.01479</v>
       </c>
       <c r="H4">
         <v>0.10399</v>
       </c>
       <c r="I4">
-        <v>5.4200000000000003E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>1</v>
       </c>
@@ -557,7 +531,7 @@
         <v>0.02</v>
       </c>
       <c r="D5">
-        <v>173.51599999999999</v>
+        <v>173.516</v>
       </c>
       <c r="E5">
         <v>-1.462</v>
@@ -566,16 +540,16 @@
         <v>164.19</v>
       </c>
       <c r="G5">
-        <v>1.5100000000000001E-2</v>
+        <v>0.0151</v>
       </c>
       <c r="H5">
-        <v>0.10394200000000001</v>
+        <v>0.103942</v>
       </c>
       <c r="I5">
-        <v>5.6800000000000002E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>2</v>
       </c>
@@ -586,7 +560,7 @@
         <v>0.02</v>
       </c>
       <c r="D6">
-        <v>173.60599999999999</v>
+        <v>173.606</v>
       </c>
       <c r="E6">
         <v>-1.46</v>
@@ -595,16 +569,16 @@
         <v>164.322</v>
       </c>
       <c r="G6">
-        <v>1.512E-2</v>
+        <v>0.01512</v>
       </c>
       <c r="H6">
-        <v>0.10394299999999999</v>
+        <v>0.103943</v>
       </c>
       <c r="I6">
-        <v>5.6699999999999997E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00567</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>3</v>
       </c>
@@ -615,25 +589,25 @@
         <v>0.02</v>
       </c>
       <c r="D7">
-        <v>173.47900000000001</v>
+        <v>173.479</v>
       </c>
       <c r="E7">
         <v>-1.466</v>
       </c>
       <c r="F7">
-        <v>164.15899999999999</v>
+        <v>164.159</v>
       </c>
       <c r="G7">
-        <v>1.5180000000000001E-2</v>
+        <v>0.01518</v>
       </c>
       <c r="H7">
         <v>0.103945</v>
       </c>
       <c r="I7">
-        <v>5.6699999999999997E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00567</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>1</v>
       </c>
@@ -653,16 +627,16 @@
         <v>103.045</v>
       </c>
       <c r="G8">
-        <v>1.6619999999999999E-2</v>
+        <v>0.01662</v>
       </c>
       <c r="H8">
         <v>0.103932</v>
       </c>
       <c r="I8">
-        <v>2.7399999999999998E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>2</v>
       </c>
@@ -673,25 +647,25 @@
         <v>0.03</v>
       </c>
       <c r="D9">
-        <v>172.79900000000001</v>
+        <v>172.799</v>
       </c>
       <c r="E9">
-        <v>-2.1779999999999999</v>
+        <v>-2.178</v>
       </c>
       <c r="F9">
-        <v>103.11199999999999</v>
+        <v>103.112</v>
       </c>
       <c r="G9">
-        <v>1.6650000000000002E-2</v>
+        <v>0.01665</v>
       </c>
       <c r="H9">
-        <v>0.10392700000000001</v>
+        <v>0.103927</v>
       </c>
       <c r="I9">
-        <v>2.7100000000000002E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>3</v>
       </c>
@@ -705,22 +679,22 @@
         <v>172.697</v>
       </c>
       <c r="E10">
-        <v>-2.1749999999999998</v>
+        <v>-2.175</v>
       </c>
       <c r="F10">
         <v>103.129</v>
       </c>
       <c r="G10">
-        <v>1.67E-2</v>
+        <v>0.0167</v>
       </c>
       <c r="H10">
         <v>0.103938</v>
       </c>
       <c r="I10">
-        <v>2.7499999999999998E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>1</v>
       </c>
@@ -731,25 +705,25 @@
         <v>0.04</v>
       </c>
       <c r="D11">
-        <v>172.46100000000001</v>
+        <v>172.461</v>
       </c>
       <c r="E11">
-        <v>-2.8839999999999999</v>
+        <v>-2.884</v>
       </c>
       <c r="F11">
-        <v>143.13800000000001</v>
+        <v>143.138</v>
       </c>
       <c r="G11">
-        <v>1.516E-2</v>
+        <v>0.01516</v>
       </c>
       <c r="H11">
         <v>0.103907</v>
       </c>
       <c r="I11">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>2</v>
       </c>
@@ -763,22 +737,22 @@
         <v>172.542</v>
       </c>
       <c r="E12">
-        <v>-2.8879999999999999</v>
+        <v>-2.888</v>
       </c>
       <c r="F12">
-        <v>143.67099999999999</v>
+        <v>143.671</v>
       </c>
       <c r="G12">
-        <v>1.5180000000000001E-2</v>
+        <v>0.01518</v>
       </c>
       <c r="H12">
-        <v>0.10391300000000001</v>
+        <v>0.103913</v>
       </c>
       <c r="I12">
-        <v>3.0100000000000001E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>3</v>
       </c>
@@ -789,25 +763,25 @@
         <v>0.04</v>
       </c>
       <c r="D13">
-        <v>172.43899999999999</v>
+        <v>172.439</v>
       </c>
       <c r="E13">
-        <v>-2.8849999999999998</v>
+        <v>-2.885</v>
       </c>
       <c r="F13">
         <v>143.334</v>
       </c>
       <c r="G13">
-        <v>1.524E-2</v>
+        <v>0.01524</v>
       </c>
       <c r="H13">
         <v>0.103923</v>
       </c>
       <c r="I13">
-        <v>3.0400000000000002E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>1</v>
       </c>
@@ -818,25 +792,25 @@
         <v>0.05</v>
       </c>
       <c r="D14">
-        <v>176.49799999999999</v>
+        <v>176.498</v>
       </c>
       <c r="E14">
-        <v>-3.6019999999999999</v>
+        <v>-3.602</v>
       </c>
       <c r="F14">
-        <v>154.46600000000001</v>
+        <v>154.466</v>
       </c>
       <c r="G14">
-        <v>1.4149999999999999E-2</v>
+        <v>0.01415</v>
       </c>
       <c r="H14">
         <v>0.103903</v>
       </c>
       <c r="I14">
-        <v>4.0600000000000002E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00406</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>2</v>
       </c>
@@ -847,25 +821,25 @@
         <v>0.05</v>
       </c>
       <c r="D15">
-        <v>176.64500000000001</v>
+        <v>176.645</v>
       </c>
       <c r="E15">
-        <v>-3.6059999999999999</v>
+        <v>-3.606</v>
       </c>
       <c r="F15">
-        <v>154.75299999999999</v>
+        <v>154.753</v>
       </c>
       <c r="G15">
-        <v>1.417E-2</v>
+        <v>0.01417</v>
       </c>
       <c r="H15">
         <v>0.103897</v>
       </c>
       <c r="I15">
-        <v>4.0499999999999998E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>3</v>
       </c>
@@ -876,25 +850,25 @@
         <v>0.05</v>
       </c>
       <c r="D16">
-        <v>176.50899999999999</v>
+        <v>176.509</v>
       </c>
       <c r="E16">
         <v>-3.613</v>
       </c>
       <c r="F16">
-        <v>154.40799999999999</v>
+        <v>154.408</v>
       </c>
       <c r="G16">
-        <v>1.4200000000000001E-2</v>
+        <v>0.0142</v>
       </c>
       <c r="H16">
-        <v>0.10391400000000001</v>
+        <v>0.103914</v>
       </c>
       <c r="I16">
-        <v>4.0699999999999998E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00407</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>1</v>
       </c>
@@ -908,22 +882,22 @@
         <v>175.1</v>
       </c>
       <c r="E17">
-        <v>-4.3129999999999997</v>
+        <v>-4.313</v>
       </c>
       <c r="F17">
         <v>146.435</v>
       </c>
       <c r="G17">
-        <v>1.405E-2</v>
+        <v>0.01405</v>
       </c>
       <c r="H17">
         <v>0.103897</v>
       </c>
       <c r="I17">
-        <v>4.8500000000000001E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00485</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>2</v>
       </c>
@@ -937,22 +911,22 @@
         <v>175.25</v>
       </c>
       <c r="E18">
-        <v>-4.3129999999999997</v>
+        <v>-4.313</v>
       </c>
       <c r="F18">
-        <v>146.50700000000001</v>
+        <v>146.507</v>
       </c>
       <c r="G18">
-        <v>1.4069999999999999E-2</v>
+        <v>0.01407</v>
       </c>
       <c r="H18">
         <v>0.103904</v>
       </c>
       <c r="I18">
-        <v>4.8399999999999997E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00484</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>3</v>
       </c>
@@ -963,25 +937,25 @@
         <v>0.06</v>
       </c>
       <c r="D19">
-        <v>175.08600000000001</v>
+        <v>175.086</v>
       </c>
       <c r="E19">
-        <v>-4.3209999999999997</v>
+        <v>-4.321</v>
       </c>
       <c r="F19">
-        <v>146.46899999999999</v>
+        <v>146.469</v>
       </c>
       <c r="G19">
-        <v>1.41E-2</v>
+        <v>0.0141</v>
       </c>
       <c r="H19">
-        <v>0.10391499999999999</v>
+        <v>0.103915</v>
       </c>
       <c r="I19">
-        <v>4.8599999999999997E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00486</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>1</v>
       </c>
@@ -989,28 +963,28 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="D20">
         <v>171.376</v>
       </c>
       <c r="E20">
-        <v>-5.0330000000000004</v>
+        <v>-5.033</v>
       </c>
       <c r="F20">
-        <v>161.57300000000001</v>
+        <v>161.573</v>
       </c>
       <c r="G20">
-        <v>1.3429999999999999E-2</v>
+        <v>0.01343</v>
       </c>
       <c r="H20">
         <v>0.103892</v>
       </c>
       <c r="I20">
-        <v>5.0200000000000002E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00502</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1018,28 +992,28 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="D21">
         <v>171.501</v>
       </c>
       <c r="E21">
-        <v>-5.0309999999999997</v>
+        <v>-5.031</v>
       </c>
       <c r="F21">
-        <v>161.89400000000001</v>
+        <v>161.894</v>
       </c>
       <c r="G21">
-        <v>1.3429999999999999E-2</v>
+        <v>0.01343</v>
       </c>
       <c r="H21">
         <v>0.103903</v>
       </c>
       <c r="I21">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1047,28 +1021,28 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="D22">
-        <v>171.25700000000001</v>
+        <v>171.257</v>
       </c>
       <c r="E22">
         <v>-5.04</v>
       </c>
       <c r="F22">
-        <v>161.54900000000001</v>
+        <v>161.549</v>
       </c>
       <c r="G22">
-        <v>1.349E-2</v>
+        <v>0.01349</v>
       </c>
       <c r="H22">
-        <v>0.10392700000000001</v>
+        <v>0.103927</v>
       </c>
       <c r="I22">
-        <v>5.0499999999999998E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00505</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1079,7 +1053,7 @@
         <v>0.08</v>
       </c>
       <c r="D23">
-        <v>168.91200000000001</v>
+        <v>168.912</v>
       </c>
       <c r="E23">
         <v>-5.75</v>
@@ -1088,16 +1062,16 @@
         <v>154.649</v>
       </c>
       <c r="G23">
-        <v>1.431E-2</v>
+        <v>0.01431</v>
       </c>
       <c r="H23">
-        <v>0.10388799999999999</v>
+        <v>0.103888</v>
       </c>
       <c r="I23">
-        <v>4.7299999999999998E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00473</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1111,22 +1085,22 @@
         <v>169.214</v>
       </c>
       <c r="E24">
-        <v>-5.7469999999999999</v>
+        <v>-5.747</v>
       </c>
       <c r="F24">
         <v>154.989</v>
       </c>
       <c r="G24">
-        <v>1.431E-2</v>
+        <v>0.01431</v>
       </c>
       <c r="H24">
         <v>0.103897</v>
       </c>
       <c r="I24">
-        <v>4.6699999999999997E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00467</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1137,25 +1111,25 @@
         <v>0.08</v>
       </c>
       <c r="D25">
-        <v>168.94900000000001</v>
+        <v>168.949</v>
       </c>
       <c r="E25">
-        <v>-5.7450000000000001</v>
+        <v>-5.745</v>
       </c>
       <c r="F25">
         <v>154.667</v>
       </c>
       <c r="G25">
-        <v>1.438E-2</v>
+        <v>0.01438</v>
       </c>
       <c r="H25">
-        <v>0.10391599999999999</v>
+        <v>0.103916</v>
       </c>
       <c r="I25">
-        <v>4.7600000000000003E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00476</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1169,22 +1143,22 @@
         <v>168.328</v>
       </c>
       <c r="E26">
-        <v>-6.4669999999999996</v>
+        <v>-6.467</v>
       </c>
       <c r="F26">
         <v>145.077</v>
       </c>
       <c r="G26">
-        <v>1.529E-2</v>
+        <v>0.01529</v>
       </c>
       <c r="H26">
         <v>0.103894</v>
       </c>
       <c r="I26">
-        <v>4.8700000000000002E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00487</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1195,25 +1169,25 @@
         <v>0.09</v>
       </c>
       <c r="D27">
-        <v>168.49799999999999</v>
+        <v>168.498</v>
       </c>
       <c r="E27">
-        <v>-6.4630000000000001</v>
+        <v>-6.463</v>
       </c>
       <c r="F27">
-        <v>145.10599999999999</v>
+        <v>145.106</v>
       </c>
       <c r="G27">
-        <v>1.529E-2</v>
+        <v>0.01529</v>
       </c>
       <c r="H27">
         <v>0.103906</v>
       </c>
       <c r="I27">
-        <v>4.8500000000000001E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00485</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1224,25 +1198,25 @@
         <v>0.09</v>
       </c>
       <c r="D28">
-        <v>168.38900000000001</v>
+        <v>168.389</v>
       </c>
       <c r="E28">
-        <v>-6.4669999999999996</v>
+        <v>-6.467</v>
       </c>
       <c r="F28">
         <v>145.238</v>
       </c>
       <c r="G28">
-        <v>1.5389999999999999E-2</v>
+        <v>0.01539</v>
       </c>
       <c r="H28">
-        <v>0.10391599999999999</v>
+        <v>0.103916</v>
       </c>
       <c r="I28">
-        <v>4.9199999999999999E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00492</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1253,25 +1227,25 @@
         <v>0.1</v>
       </c>
       <c r="D29">
-        <v>168.55699999999999</v>
+        <v>168.557</v>
       </c>
       <c r="E29">
-        <v>-7.1749999999999998</v>
+        <v>-7.175</v>
       </c>
       <c r="F29">
         <v>139.965</v>
       </c>
       <c r="G29">
-        <v>1.5219999999999999E-2</v>
+        <v>0.01522</v>
       </c>
       <c r="H29">
         <v>0.10388</v>
       </c>
       <c r="I29">
-        <v>5.1700000000000001E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00517</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1282,25 +1256,25 @@
         <v>0.1</v>
       </c>
       <c r="D30">
-        <v>168.69800000000001</v>
+        <v>168.698</v>
       </c>
       <c r="E30">
-        <v>-7.1820000000000004</v>
+        <v>-7.182</v>
       </c>
       <c r="F30">
         <v>139.976</v>
       </c>
       <c r="G30">
-        <v>1.519E-2</v>
+        <v>0.01519</v>
       </c>
       <c r="H30">
         <v>0.103892</v>
       </c>
       <c r="I30">
-        <v>5.1200000000000004E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00512</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1311,25 +1285,25 @@
         <v>0.1</v>
       </c>
       <c r="D31">
-        <v>168.58099999999999</v>
+        <v>168.581</v>
       </c>
       <c r="E31">
-        <v>-7.1779999999999999</v>
+        <v>-7.178</v>
       </c>
       <c r="F31">
         <v>140.28</v>
       </c>
       <c r="G31">
-        <v>1.528E-2</v>
+        <v>0.01528</v>
       </c>
       <c r="H31">
         <v>0.103912</v>
       </c>
       <c r="I31">
-        <v>5.1900000000000002E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00519</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1349,16 +1323,16 @@
         <v>123.989</v>
       </c>
       <c r="G32">
-        <v>1.4959999999999999E-2</v>
+        <v>0.01496</v>
       </c>
       <c r="H32">
         <v>0.103842</v>
       </c>
       <c r="I32">
-        <v>5.4400000000000004E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00544</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1369,7 +1343,7 @@
         <v>0.2</v>
       </c>
       <c r="D33">
-        <v>159.43299999999999</v>
+        <v>159.433</v>
       </c>
       <c r="E33">
         <v>-14.308</v>
@@ -1378,16 +1352,16 @@
         <v>124.12</v>
       </c>
       <c r="G33">
-        <v>1.4959999999999999E-2</v>
+        <v>0.01496</v>
       </c>
       <c r="H33">
         <v>0.103821</v>
       </c>
       <c r="I33">
-        <v>5.4200000000000003E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00542</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1398,25 +1372,25 @@
         <v>0.2</v>
       </c>
       <c r="D34">
-        <v>159.32900000000001</v>
+        <v>159.329</v>
       </c>
       <c r="E34">
         <v>-14.315</v>
       </c>
       <c r="F34">
-        <v>123.78700000000001</v>
+        <v>123.787</v>
       </c>
       <c r="G34">
-        <v>1.5010000000000001E-2</v>
+        <v>0.01501</v>
       </c>
       <c r="H34">
-        <v>0.10383100000000001</v>
+        <v>0.103831</v>
       </c>
       <c r="I34">
-        <v>5.4200000000000003E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00542</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1427,25 +1401,25 @@
         <v>0.3</v>
       </c>
       <c r="D35">
-        <v>151.46799999999999</v>
+        <v>151.468</v>
       </c>
       <c r="E35">
         <v>-21.448</v>
       </c>
       <c r="F35">
-        <v>110.40600000000001</v>
+        <v>110.406</v>
       </c>
       <c r="G35">
-        <v>1.524E-2</v>
+        <v>0.01524</v>
       </c>
       <c r="H35">
         <v>0.103742</v>
       </c>
       <c r="I35">
-        <v>6.0400000000000002E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1465,16 +1439,16 @@
         <v>110.28</v>
       </c>
       <c r="G36">
-        <v>1.525E-2</v>
+        <v>0.01525</v>
       </c>
       <c r="H36">
-        <v>0.10376299999999999</v>
+        <v>0.103763</v>
       </c>
       <c r="I36">
-        <v>6.0200000000000002E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00602</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1485,25 +1459,25 @@
         <v>0.3</v>
       </c>
       <c r="D37">
-        <v>151.59299999999999</v>
+        <v>151.593</v>
       </c>
       <c r="E37">
-        <v>-21.449000000000002</v>
+        <v>-21.449</v>
       </c>
       <c r="F37">
-        <v>110.45399999999999</v>
+        <v>110.454</v>
       </c>
       <c r="G37">
-        <v>1.528E-2</v>
+        <v>0.01528</v>
       </c>
       <c r="H37">
         <v>0.103752</v>
       </c>
       <c r="I37">
-        <v>6.0499999999999998E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00605</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1517,22 +1491,22 @@
         <v>143.078</v>
       </c>
       <c r="E38">
-        <v>-28.571999999999999</v>
+        <v>-28.572</v>
       </c>
       <c r="F38">
-        <v>97.063999999999993</v>
+        <v>97.064</v>
       </c>
       <c r="G38">
-        <v>1.5219999999999999E-2</v>
+        <v>0.01522</v>
       </c>
       <c r="H38">
         <v>0.103746</v>
       </c>
       <c r="I38">
-        <v>7.6099999999999996E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00761</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1546,22 +1520,22 @@
         <v>143.107</v>
       </c>
       <c r="E39">
-        <v>-28.571999999999999</v>
+        <v>-28.572</v>
       </c>
       <c r="F39">
-        <v>96.921999999999997</v>
+        <v>96.922</v>
       </c>
       <c r="G39">
-        <v>1.5219999999999999E-2</v>
+        <v>0.01522</v>
       </c>
       <c r="H39">
         <v>0.103741</v>
       </c>
       <c r="I39">
-        <v>7.5900000000000004E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00759</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1572,25 +1546,25 @@
         <v>0.4</v>
       </c>
       <c r="D40">
-        <v>142.88300000000001</v>
+        <v>142.883</v>
       </c>
       <c r="E40">
         <v>-28.567</v>
       </c>
       <c r="F40">
-        <v>96.587999999999994</v>
+        <v>96.588</v>
       </c>
       <c r="G40">
-        <v>1.524E-2</v>
+        <v>0.01524</v>
       </c>
       <c r="H40">
-        <v>0.10374800000000001</v>
+        <v>0.103748</v>
       </c>
       <c r="I40">
-        <v>7.5599999999999999E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00756</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1604,22 +1578,22 @@
         <v>134.221</v>
       </c>
       <c r="E41">
-        <v>-35.692999999999998</v>
+        <v>-35.693</v>
       </c>
       <c r="F41">
-        <v>82.161000000000001</v>
+        <v>82.161</v>
       </c>
       <c r="G41">
-        <v>1.5570000000000001E-2</v>
+        <v>0.01557</v>
       </c>
       <c r="H41">
         <v>0.103695</v>
       </c>
       <c r="I41">
-        <v>8.4100000000000008E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00841</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1636,19 +1610,19 @@
         <v>-35.695</v>
       </c>
       <c r="F42">
-        <v>82.316999999999993</v>
+        <v>82.317</v>
       </c>
       <c r="G42">
-        <v>1.555E-2</v>
+        <v>0.01555</v>
       </c>
       <c r="H42">
         <v>0.10369</v>
       </c>
       <c r="I42">
-        <v>8.3899999999999999E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00839</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>3</v>
       </c>
@@ -1659,25 +1633,25 @@
         <v>0.5</v>
       </c>
       <c r="D43">
-        <v>134.27600000000001</v>
+        <v>134.276</v>
       </c>
       <c r="E43">
-        <v>-35.697000000000003</v>
+        <v>-35.697</v>
       </c>
       <c r="F43">
-        <v>82.602000000000004</v>
+        <v>82.602</v>
       </c>
       <c r="G43">
-        <v>1.558E-2</v>
+        <v>0.01558</v>
       </c>
       <c r="H43">
         <v>0.103686</v>
       </c>
       <c r="I43">
-        <v>8.3899999999999999E-3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00839</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1688,25 +1662,25 @@
         <v>0.6</v>
       </c>
       <c r="D44">
-        <v>127.22799999999999</v>
+        <v>127.228</v>
       </c>
       <c r="E44">
         <v>-42.82</v>
       </c>
       <c r="F44">
-        <v>77.552000000000007</v>
+        <v>77.552</v>
       </c>
       <c r="G44">
-        <v>1.644E-2</v>
+        <v>0.01644</v>
       </c>
       <c r="H44">
         <v>0.103612</v>
       </c>
       <c r="I44">
-        <v>9.6900000000000007E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00969</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1720,22 +1694,22 @@
         <v>127.274</v>
       </c>
       <c r="E45">
-        <v>-42.811999999999998</v>
+        <v>-42.812</v>
       </c>
       <c r="F45">
-        <v>77.472999999999999</v>
+        <v>77.473</v>
       </c>
       <c r="G45">
-        <v>1.6469999999999999E-2</v>
+        <v>0.01647</v>
       </c>
       <c r="H45">
-        <v>0.10362200000000001</v>
+        <v>0.103622</v>
       </c>
       <c r="I45">
-        <v>9.7199999999999995E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00972</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>3</v>
       </c>
@@ -1746,25 +1720,25 @@
         <v>0.6</v>
       </c>
       <c r="D46">
-        <v>127.18899999999999</v>
+        <v>127.189</v>
       </c>
       <c r="E46">
-        <v>-42.814999999999998</v>
+        <v>-42.815</v>
       </c>
       <c r="F46">
-        <v>77.287000000000006</v>
+        <v>77.287</v>
       </c>
       <c r="G46">
-        <v>1.6469999999999999E-2</v>
+        <v>0.01647</v>
       </c>
       <c r="H46">
         <v>0.103615</v>
       </c>
       <c r="I46">
-        <v>9.7199999999999995E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.00972</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>1</v>
       </c>
@@ -1781,19 +1755,19 @@
         <v>-49.927</v>
       </c>
       <c r="F47">
-        <v>63.039000000000001</v>
+        <v>63.039</v>
       </c>
       <c r="G47">
-        <v>1.6930000000000001E-2</v>
+        <v>0.01693</v>
       </c>
       <c r="H47">
-        <v>0.10360800000000001</v>
+        <v>0.103608</v>
       </c>
       <c r="I47">
-        <v>1.137E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1807,22 +1781,22 @@
         <v>121.477</v>
       </c>
       <c r="E48">
-        <v>-49.926000000000002</v>
+        <v>-49.926</v>
       </c>
       <c r="F48">
-        <v>62.981000000000002</v>
+        <v>62.981</v>
       </c>
       <c r="G48">
-        <v>1.6899999999999998E-2</v>
+        <v>0.0169</v>
       </c>
       <c r="H48">
         <v>0.103601</v>
       </c>
       <c r="I48">
-        <v>1.1339999999999999E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>3</v>
       </c>
@@ -1836,22 +1810,22 @@
         <v>121.407</v>
       </c>
       <c r="E49">
-        <v>-49.924999999999997</v>
+        <v>-49.925</v>
       </c>
       <c r="F49">
-        <v>63.158000000000001</v>
+        <v>63.158</v>
       </c>
       <c r="G49">
-        <v>1.6910000000000001E-2</v>
+        <v>0.01691</v>
       </c>
       <c r="H49">
         <v>0.103592</v>
       </c>
       <c r="I49">
-        <v>1.132E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1868,19 +1842,19 @@
         <v>-57.055</v>
       </c>
       <c r="F50">
-        <v>64.534000000000006</v>
+        <v>64.534</v>
       </c>
       <c r="G50">
-        <v>1.7420000000000001E-2</v>
+        <v>0.01742</v>
       </c>
       <c r="H50">
         <v>0.103577</v>
       </c>
       <c r="I50">
-        <v>1.157E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>2</v>
       </c>
@@ -1891,25 +1865,25 @@
         <v>0.8</v>
       </c>
       <c r="D51">
-        <v>115.35599999999999</v>
+        <v>115.356</v>
       </c>
       <c r="E51">
-        <v>-57.051000000000002</v>
+        <v>-57.051</v>
       </c>
       <c r="F51">
-        <v>64.465999999999994</v>
+        <v>64.466</v>
       </c>
       <c r="G51">
-        <v>1.7409999999999998E-2</v>
+        <v>0.01741</v>
       </c>
       <c r="H51">
-        <v>0.10358000000000001</v>
+        <v>0.10358</v>
       </c>
       <c r="I51">
-        <v>1.157E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52">
         <v>3</v>
       </c>
@@ -1923,22 +1897,22 @@
         <v>115.294</v>
       </c>
       <c r="E52">
-        <v>-57.045000000000002</v>
+        <v>-57.045</v>
       </c>
       <c r="F52">
-        <v>64.343999999999994</v>
+        <v>64.344</v>
       </c>
       <c r="G52">
-        <v>1.7389999999999999E-2</v>
+        <v>0.01739</v>
       </c>
       <c r="H52">
         <v>0.103576</v>
       </c>
       <c r="I52">
-        <v>1.159E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53">
         <v>1</v>
       </c>
@@ -1952,22 +1926,22 @@
         <v>107.91</v>
       </c>
       <c r="E53">
-        <v>-64.156000000000006</v>
+        <v>-64.156</v>
       </c>
       <c r="F53">
-        <v>48.290999999999997</v>
+        <v>48.291</v>
       </c>
       <c r="G53">
-        <v>1.779E-2</v>
+        <v>0.01779</v>
       </c>
       <c r="H53">
         <v>0.103508</v>
       </c>
       <c r="I53">
-        <v>1.366E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01366</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54">
         <v>2</v>
       </c>
@@ -1981,22 +1955,22 @@
         <v>107.943</v>
       </c>
       <c r="E54">
-        <v>-64.149000000000001</v>
+        <v>-64.149</v>
       </c>
       <c r="F54">
         <v>48.192</v>
       </c>
       <c r="G54">
-        <v>1.7819999999999999E-2</v>
+        <v>0.01782</v>
       </c>
       <c r="H54">
         <v>0.103515</v>
       </c>
       <c r="I54">
-        <v>1.367E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01367</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55">
         <v>3</v>
       </c>
@@ -2007,25 +1981,25 @@
         <v>0.9</v>
       </c>
       <c r="D55">
-        <v>107.95099999999999</v>
+        <v>107.951</v>
       </c>
       <c r="E55">
-        <v>-64.152000000000001</v>
+        <v>-64.152</v>
       </c>
       <c r="F55">
-        <v>48.051000000000002</v>
+        <v>48.051</v>
       </c>
       <c r="G55">
-        <v>1.7819999999999999E-2</v>
+        <v>0.01782</v>
       </c>
       <c r="H55">
         <v>0.103503</v>
       </c>
       <c r="I55">
-        <v>1.366E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01366</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2039,22 +2013,22 @@
         <v>101.807</v>
       </c>
       <c r="E56">
-        <v>-71.239000000000004</v>
+        <v>-71.239</v>
       </c>
       <c r="F56">
-        <v>46.268999999999998</v>
+        <v>46.269</v>
       </c>
       <c r="G56">
-        <v>1.9009999999999999E-2</v>
+        <v>0.01901</v>
       </c>
       <c r="H56">
-        <v>0.10345500000000001</v>
+        <v>0.103455</v>
       </c>
       <c r="I56">
-        <v>1.3339999999999999E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01334</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57">
         <v>2</v>
       </c>
@@ -2065,25 +2039,25 @@
         <v>1</v>
       </c>
       <c r="D57">
-        <v>101.86799999999999</v>
+        <v>101.868</v>
       </c>
       <c r="E57">
-        <v>-71.242000000000004</v>
+        <v>-71.242</v>
       </c>
       <c r="F57">
-        <v>46.323999999999998</v>
+        <v>46.324</v>
       </c>
       <c r="G57">
-        <v>1.8970000000000001E-2</v>
+        <v>0.01897</v>
       </c>
       <c r="H57">
-        <v>0.10345500000000001</v>
+        <v>0.103455</v>
       </c>
       <c r="I57">
-        <v>1.3350000000000001E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.01335</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>3</v>
       </c>
@@ -2097,22 +2071,22 @@
         <v>101.783</v>
       </c>
       <c r="E58">
-        <v>-71.236000000000004</v>
+        <v>-71.236</v>
       </c>
       <c r="F58">
-        <v>46.273000000000003</v>
+        <v>46.273</v>
       </c>
       <c r="G58">
-        <v>1.8929999999999999E-2</v>
+        <v>0.01893</v>
       </c>
       <c r="H58">
         <v>0.103466</v>
       </c>
       <c r="I58">
-        <v>1.337E-2</v>
+        <v>0.01337</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>